<commit_message>
Logic of the program is endeed. The programs now is able to find and validate the existence before register the unity
</commit_message>
<xml_diff>
--- a/model/test_sheet.xlsx
+++ b/model/test_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SgdCad\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAC37F0-2798-4FED-B98E-071837FA778A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D3F9FE-AF87-4B5B-A645-4EB4FE28BF47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>POLOS</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>EAD CAMPO VERDE - JARDIM CAMPO VERDE - MT</t>
+  </si>
+  <si>
+    <t>teste1</t>
+  </si>
+  <si>
+    <t>testeIES1</t>
+  </si>
+  <si>
+    <t>teste2</t>
+  </si>
+  <si>
+    <t>testeIES2</t>
   </si>
 </sst>
 </file>
@@ -132,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -215,11 +227,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -245,6 +283,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -558,60 +602,48 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>2042</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="4">
         <v>1742</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="7">
-        <v>374</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1624</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="7">
-        <v>374</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1751</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
+    <row r="4" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7">
         <v>374</v>
@@ -620,66 +652,66 @@
         <v>8</v>
       </c>
       <c r="D5" s="7">
-        <v>1621</v>
+        <v>1624</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="7">
-        <v>610</v>
+        <v>374</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="7">
-        <v>1686</v>
+        <v>1751</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="8">
-        <v>610</v>
+        <v>10</v>
+      </c>
+      <c r="B7" s="7">
+        <v>374</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
-        <v>1708</v>
+        <v>1621</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A8" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="7">
-        <v>374</v>
+        <v>610</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D8" s="7">
-        <v>1822</v>
+        <v>1686</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A9" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="8">
         <v>610</v>
@@ -688,15 +720,15 @@
         <v>12</v>
       </c>
       <c r="D9" s="7">
-        <v>1712</v>
+        <v>1708</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="7">
         <v>374</v>
@@ -705,32 +737,32 @@
         <v>8</v>
       </c>
       <c r="D10" s="7">
-        <v>1732</v>
+        <v>1822</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="7">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8">
         <v>610</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="7">
-        <v>1500</v>
+        <v>1712</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A12" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="7">
         <v>374</v>
@@ -739,15 +771,15 @@
         <v>8</v>
       </c>
       <c r="D12" s="7">
-        <v>1838</v>
+        <v>1732</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A13" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="7">
         <v>610</v>
@@ -756,43 +788,77 @@
         <v>12</v>
       </c>
       <c r="D13" s="7">
-        <v>1715</v>
+        <v>1500</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="7">
         <v>374</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="4">
-        <v>366</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>20</v>
+      <c r="D14" s="7">
+        <v>1838</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="7">
+        <v>610</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1715</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4">
+        <v>374</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4">
+        <v>366</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B17" s="7">
         <v>374</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D17" s="7">
         <v>1857</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>